<commit_message>
C6 - Edit Training_Git.xlxs
</commit_message>
<xml_diff>
--- a/Training_Git.xlsx
+++ b/Training_Git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DocumentExample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901D9530-9540-4C64-AC6D-F2EFE6F13AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209E7CA8-248A-49B7-91AD-B1FD25F365AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-2160" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -801,24 +801,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -902,6 +884,24 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1638,9 +1638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC140"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A118" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="T124" sqref="T124"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="15"/>
   <cols>
@@ -1655,93 +1653,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="14.25">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="46"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
+      <c r="AB1" s="74"/>
     </row>
     <row r="2" spans="2:28" ht="14.25">
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="49"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="76"/>
+      <c r="W2" s="76"/>
+      <c r="X2" s="76"/>
+      <c r="Y2" s="76"/>
+      <c r="Z2" s="76"/>
+      <c r="AA2" s="76"/>
+      <c r="AB2" s="77"/>
     </row>
     <row r="3" spans="2:28" ht="14.25">
-      <c r="B3" s="47"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
-      <c r="T3" s="48"/>
-      <c r="U3" s="48"/>
-      <c r="V3" s="48"/>
-      <c r="W3" s="48"/>
-      <c r="X3" s="48"/>
-      <c r="Y3" s="48"/>
-      <c r="Z3" s="48"/>
-      <c r="AA3" s="48"/>
-      <c r="AB3" s="49"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="76"/>
+      <c r="AB3" s="77"/>
     </row>
     <row r="4" spans="2:28" ht="20.100000000000001" customHeight="1">
       <c r="B4" s="4"/>
@@ -2121,10 +2119,10 @@
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="30"/>
-      <c r="E16" s="52" t="s">
+      <c r="E16" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="51" t="s">
+      <c r="F16" s="45" t="s">
         <v>38</v>
       </c>
       <c r="G16" s="15"/>
@@ -2154,7 +2152,7 @@
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="30"/>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="47" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="16" t="s">
@@ -2187,7 +2185,7 @@
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="30"/>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="47" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="17" t="s">
@@ -3826,7 +3824,7 @@
       <c r="C74" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D74" s="66" t="s">
+      <c r="D74" s="60" t="s">
         <v>55</v>
       </c>
       <c r="E74" s="5"/>
@@ -3920,7 +3918,7 @@
       <c r="B77" s="6"/>
       <c r="C77" s="7"/>
       <c r="D77" s="30"/>
-      <c r="E77" s="50" t="s">
+      <c r="E77" s="44" t="s">
         <v>3</v>
       </c>
       <c r="F77" s="24" t="s">
@@ -4052,7 +4050,7 @@
       <c r="B81" s="6"/>
       <c r="C81" s="7"/>
       <c r="D81" s="30"/>
-      <c r="E81" s="50" t="s">
+      <c r="E81" s="44" t="s">
         <v>3</v>
       </c>
       <c r="F81" s="24" t="s">
@@ -4085,7 +4083,7 @@
       <c r="B82" s="6"/>
       <c r="C82" s="7"/>
       <c r="D82" s="32"/>
-      <c r="E82" s="50" t="s">
+      <c r="E82" s="44" t="s">
         <v>3</v>
       </c>
       <c r="F82" s="24" t="s">
@@ -4118,7 +4116,7 @@
       <c r="B83" s="6"/>
       <c r="C83" s="7"/>
       <c r="D83" s="30"/>
-      <c r="E83" s="50" t="s">
+      <c r="E83" s="44" t="s">
         <v>3</v>
       </c>
       <c r="F83" s="24" t="s">
@@ -4215,7 +4213,7 @@
       <c r="D86" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="E86" s="54" t="s">
+      <c r="E86" s="48" t="s">
         <v>39</v>
       </c>
       <c r="F86" s="8"/>
@@ -4246,10 +4244,10 @@
       <c r="B87" s="6"/>
       <c r="C87" s="7"/>
       <c r="D87" s="8"/>
-      <c r="E87" s="59" t="s">
+      <c r="E87" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F87" s="58" t="s">
+      <c r="F87" s="52" t="s">
         <v>40</v>
       </c>
       <c r="G87" s="30"/>
@@ -4282,7 +4280,7 @@
       <c r="E88" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F88" s="60" t="s">
+      <c r="F88" s="54" t="s">
         <v>41</v>
       </c>
       <c r="G88" s="30"/>
@@ -4312,30 +4310,30 @@
       <c r="B89" s="6"/>
       <c r="C89" s="7"/>
       <c r="D89" s="8"/>
-      <c r="E89" s="59" t="s">
+      <c r="E89" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F89" s="58" t="s">
+      <c r="F89" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="G89" s="56"/>
-      <c r="H89" s="57"/>
-      <c r="I89" s="57"/>
-      <c r="J89" s="57"/>
-      <c r="K89" s="57"/>
-      <c r="L89" s="57"/>
-      <c r="M89" s="57"/>
-      <c r="N89" s="57"/>
-      <c r="O89" s="57"/>
-      <c r="P89" s="57"/>
-      <c r="Q89" s="57"/>
-      <c r="R89" s="57"/>
-      <c r="S89" s="57"/>
-      <c r="T89" s="57"/>
-      <c r="U89" s="57"/>
-      <c r="V89" s="57"/>
-      <c r="W89" s="57"/>
-      <c r="X89" s="57"/>
+      <c r="G89" s="50"/>
+      <c r="H89" s="51"/>
+      <c r="I89" s="51"/>
+      <c r="J89" s="51"/>
+      <c r="K89" s="51"/>
+      <c r="L89" s="51"/>
+      <c r="M89" s="51"/>
+      <c r="N89" s="51"/>
+      <c r="O89" s="51"/>
+      <c r="P89" s="51"/>
+      <c r="Q89" s="51"/>
+      <c r="R89" s="51"/>
+      <c r="S89" s="51"/>
+      <c r="T89" s="51"/>
+      <c r="U89" s="51"/>
+      <c r="V89" s="51"/>
+      <c r="W89" s="51"/>
+      <c r="X89" s="51"/>
       <c r="Y89" s="30"/>
       <c r="Z89" s="30"/>
       <c r="AA89" s="30"/>
@@ -4345,30 +4343,30 @@
       <c r="B90" s="6"/>
       <c r="C90" s="7"/>
       <c r="D90" s="8"/>
-      <c r="E90" s="61" t="s">
+      <c r="E90" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="F90" s="60" t="s">
+      <c r="F90" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G90" s="56"/>
-      <c r="H90" s="57"/>
-      <c r="I90" s="57"/>
-      <c r="J90" s="57"/>
-      <c r="K90" s="57"/>
-      <c r="L90" s="57"/>
-      <c r="M90" s="57"/>
-      <c r="N90" s="57"/>
-      <c r="O90" s="57"/>
-      <c r="P90" s="57"/>
-      <c r="Q90" s="57"/>
-      <c r="R90" s="57"/>
-      <c r="S90" s="57"/>
-      <c r="T90" s="57"/>
-      <c r="U90" s="57"/>
-      <c r="V90" s="57"/>
-      <c r="W90" s="57"/>
-      <c r="X90" s="57"/>
+      <c r="G90" s="50"/>
+      <c r="H90" s="51"/>
+      <c r="I90" s="51"/>
+      <c r="J90" s="51"/>
+      <c r="K90" s="51"/>
+      <c r="L90" s="51"/>
+      <c r="M90" s="51"/>
+      <c r="N90" s="51"/>
+      <c r="O90" s="51"/>
+      <c r="P90" s="51"/>
+      <c r="Q90" s="51"/>
+      <c r="R90" s="51"/>
+      <c r="S90" s="51"/>
+      <c r="T90" s="51"/>
+      <c r="U90" s="51"/>
+      <c r="V90" s="51"/>
+      <c r="W90" s="51"/>
+      <c r="X90" s="51"/>
       <c r="Y90" s="30"/>
       <c r="Z90" s="30"/>
       <c r="AA90" s="30"/>
@@ -4378,10 +4376,10 @@
       <c r="B91" s="6"/>
       <c r="C91" s="7"/>
       <c r="D91" s="8"/>
-      <c r="E91" s="59" t="s">
+      <c r="E91" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F91" s="58" t="s">
+      <c r="F91" s="52" t="s">
         <v>44</v>
       </c>
       <c r="G91" s="30"/>
@@ -4411,10 +4409,10 @@
       <c r="B92" s="6"/>
       <c r="C92" s="7"/>
       <c r="D92" s="8"/>
-      <c r="E92" s="61" t="s">
+      <c r="E92" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="F92" s="60" t="s">
+      <c r="F92" s="54" t="s">
         <v>45</v>
       </c>
       <c r="G92" s="30"/>
@@ -4503,7 +4501,7 @@
       <c r="C95" s="7"/>
       <c r="D95" s="8"/>
       <c r="E95" s="30"/>
-      <c r="F95" s="55"/>
+      <c r="F95" s="49"/>
       <c r="G95" s="30"/>
       <c r="H95" s="30"/>
       <c r="I95" s="30"/>
@@ -4590,7 +4588,7 @@
       <c r="C98" s="7"/>
       <c r="D98" s="8"/>
       <c r="E98" s="30"/>
-      <c r="F98" s="55"/>
+      <c r="F98" s="49"/>
       <c r="G98" s="30"/>
       <c r="H98" s="30"/>
       <c r="I98" s="30"/>
@@ -4677,7 +4675,7 @@
       <c r="C101" s="7"/>
       <c r="D101" s="8"/>
       <c r="E101" s="30"/>
-      <c r="F101" s="55"/>
+      <c r="F101" s="49"/>
       <c r="G101" s="30"/>
       <c r="H101" s="30"/>
       <c r="I101" s="30"/>
@@ -4764,7 +4762,7 @@
       <c r="C104" s="7"/>
       <c r="D104" s="8"/>
       <c r="E104" s="30"/>
-      <c r="F104" s="55"/>
+      <c r="F104" s="49"/>
       <c r="G104" s="30"/>
       <c r="H104" s="30"/>
       <c r="I104" s="30"/>
@@ -4851,7 +4849,7 @@
       <c r="C107" s="7"/>
       <c r="D107" s="8"/>
       <c r="E107" s="30"/>
-      <c r="F107" s="55"/>
+      <c r="F107" s="49"/>
       <c r="G107" s="30"/>
       <c r="H107" s="30"/>
       <c r="I107" s="30"/>
@@ -4907,10 +4905,10 @@
     <row r="109" spans="2:28">
       <c r="B109" s="6"/>
       <c r="C109" s="29"/>
-      <c r="D109" s="62" t="s">
+      <c r="D109" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="E109" s="54" t="s">
+      <c r="E109" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F109" s="30"/>
@@ -4941,10 +4939,10 @@
       <c r="B110" s="6"/>
       <c r="C110" s="29"/>
       <c r="D110" s="30"/>
-      <c r="E110" s="59" t="s">
+      <c r="E110" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F110" s="58" t="s">
+      <c r="F110" s="52" t="s">
         <v>47</v>
       </c>
       <c r="G110" s="28"/>
@@ -4974,16 +4972,16 @@
       <c r="B111" s="6"/>
       <c r="C111" s="29"/>
       <c r="D111" s="30"/>
-      <c r="E111" s="61" t="s">
+      <c r="E111" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="F111" s="65" t="s">
+      <c r="F111" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="G111" s="63"/>
-      <c r="H111" s="64"/>
-      <c r="I111" s="64"/>
-      <c r="J111" s="64"/>
+      <c r="G111" s="57"/>
+      <c r="H111" s="58"/>
+      <c r="I111" s="58"/>
+      <c r="J111" s="58"/>
       <c r="K111" s="30"/>
       <c r="L111" s="30"/>
       <c r="M111" s="30"/>
@@ -5007,10 +5005,10 @@
       <c r="B112" s="6"/>
       <c r="C112" s="29"/>
       <c r="D112" s="30"/>
-      <c r="E112" s="59" t="s">
+      <c r="E112" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F112" s="58" t="s">
+      <c r="F112" s="52" t="s">
         <v>49</v>
       </c>
       <c r="G112" s="28"/>
@@ -5043,13 +5041,13 @@
       <c r="E113" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F113" s="65" t="s">
+      <c r="F113" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="G113" s="63"/>
-      <c r="H113" s="64"/>
-      <c r="I113" s="64"/>
-      <c r="J113" s="64"/>
+      <c r="G113" s="57"/>
+      <c r="H113" s="58"/>
+      <c r="I113" s="58"/>
+      <c r="J113" s="58"/>
       <c r="K113" s="30"/>
       <c r="L113" s="30"/>
       <c r="M113" s="30"/>
@@ -5073,10 +5071,10 @@
       <c r="B114" s="6"/>
       <c r="C114" s="29"/>
       <c r="D114" s="30"/>
-      <c r="E114" s="59" t="s">
+      <c r="E114" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F114" s="58" t="s">
+      <c r="F114" s="52" t="s">
         <v>51</v>
       </c>
       <c r="G114" s="28"/>
@@ -5109,13 +5107,13 @@
       <c r="E115" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F115" s="65" t="s">
+      <c r="F115" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="G115" s="63"/>
-      <c r="H115" s="64"/>
-      <c r="I115" s="64"/>
-      <c r="J115" s="64"/>
+      <c r="G115" s="57"/>
+      <c r="H115" s="58"/>
+      <c r="I115" s="58"/>
+      <c r="J115" s="58"/>
       <c r="K115" s="30"/>
       <c r="L115" s="30"/>
       <c r="M115" s="30"/>
@@ -5139,10 +5137,10 @@
       <c r="B116" s="6"/>
       <c r="C116" s="29"/>
       <c r="D116" s="30"/>
-      <c r="E116" s="59" t="s">
+      <c r="E116" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F116" s="58" t="s">
+      <c r="F116" s="52" t="s">
         <v>53</v>
       </c>
       <c r="G116" s="28"/>
@@ -5175,18 +5173,18 @@
       <c r="E117" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F117" s="65" t="s">
+      <c r="F117" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="G117" s="63"/>
-      <c r="H117" s="64"/>
-      <c r="I117" s="64"/>
-      <c r="J117" s="64"/>
-      <c r="K117" s="64"/>
-      <c r="L117" s="64"/>
-      <c r="M117" s="64"/>
-      <c r="N117" s="64"/>
-      <c r="O117" s="64"/>
+      <c r="G117" s="57"/>
+      <c r="H117" s="58"/>
+      <c r="I117" s="58"/>
+      <c r="J117" s="58"/>
+      <c r="K117" s="58"/>
+      <c r="L117" s="58"/>
+      <c r="M117" s="58"/>
+      <c r="N117" s="58"/>
+      <c r="O117" s="58"/>
       <c r="P117" s="30"/>
       <c r="Q117" s="30"/>
       <c r="R117" s="30"/>
@@ -5206,8 +5204,8 @@
       <c r="C118" s="29"/>
       <c r="D118" s="30"/>
       <c r="E118" s="27"/>
-      <c r="F118" s="68"/>
-      <c r="G118" s="69"/>
+      <c r="F118" s="62"/>
+      <c r="G118" s="63"/>
       <c r="H118" s="37"/>
       <c r="I118" s="37"/>
       <c r="J118" s="37"/>
@@ -5261,10 +5259,10 @@
     </row>
     <row r="120" spans="2:28" ht="20.100000000000001" customHeight="1">
       <c r="B120" s="4"/>
-      <c r="C120" s="70" t="s">
+      <c r="C120" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="D120" s="66" t="s">
+      <c r="D120" s="60" t="s">
         <v>61</v>
       </c>
       <c r="E120" s="5"/>
@@ -5324,10 +5322,10 @@
     <row r="122" spans="2:28">
       <c r="B122" s="6"/>
       <c r="C122" s="29"/>
-      <c r="D122" s="62" t="s">
+      <c r="D122" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="E122" s="54" t="s">
+      <c r="E122" s="48" t="s">
         <v>69</v>
       </c>
       <c r="F122" s="30"/>
@@ -5357,8 +5355,8 @@
     <row r="123" spans="2:28">
       <c r="B123" s="6"/>
       <c r="C123" s="29"/>
-      <c r="D123" s="62"/>
-      <c r="E123" s="58" t="s">
+      <c r="D123" s="56"/>
+      <c r="E123" s="52" t="s">
         <v>79</v>
       </c>
       <c r="F123" s="30"/>
@@ -5389,7 +5387,7 @@
       <c r="B124" s="6"/>
       <c r="C124" s="29"/>
       <c r="D124" s="36"/>
-      <c r="E124" s="60" t="s">
+      <c r="E124" s="54" t="s">
         <v>62</v>
       </c>
       <c r="F124" s="30"/>
@@ -5405,14 +5403,14 @@
       <c r="P124" s="30"/>
       <c r="Q124" s="30"/>
       <c r="R124" s="36"/>
-      <c r="S124" s="61" t="s">
+      <c r="S124" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="T124" s="73" t="s">
+      <c r="T124" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="U124" s="74"/>
-      <c r="V124" s="74"/>
+      <c r="U124" s="68"/>
+      <c r="V124" s="68"/>
       <c r="W124" s="30"/>
       <c r="X124" s="30"/>
       <c r="Y124" s="30"/>
@@ -5424,7 +5422,7 @@
       <c r="B125" s="6"/>
       <c r="C125" s="29"/>
       <c r="D125" s="36"/>
-      <c r="E125" s="60" t="s">
+      <c r="E125" s="54" t="s">
         <v>64</v>
       </c>
       <c r="F125" s="30"/>
@@ -5456,10 +5454,10 @@
       <c r="C126" s="29"/>
       <c r="D126" s="30"/>
       <c r="E126" s="36"/>
-      <c r="F126" s="71" t="s">
+      <c r="F126" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="G126" s="72" t="s">
+      <c r="G126" s="66" t="s">
         <v>65</v>
       </c>
       <c r="H126" s="30"/>
@@ -5489,10 +5487,10 @@
       <c r="C127" s="29"/>
       <c r="D127" s="30"/>
       <c r="E127" s="36"/>
-      <c r="F127" s="61" t="s">
+      <c r="F127" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="G127" s="67" t="s">
+      <c r="G127" s="61" t="s">
         <v>66</v>
       </c>
       <c r="H127" s="30"/>
@@ -5522,13 +5520,13 @@
       <c r="C128" s="29"/>
       <c r="D128" s="30"/>
       <c r="E128" s="36"/>
-      <c r="F128" s="61" t="s">
+      <c r="F128" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="G128" s="73" t="s">
+      <c r="G128" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="H128" s="73"/>
+      <c r="H128" s="67"/>
       <c r="I128" s="30"/>
       <c r="J128" s="30"/>
       <c r="K128" s="30"/>
@@ -5555,10 +5553,10 @@
       <c r="C129" s="29"/>
       <c r="D129" s="30"/>
       <c r="E129" s="36"/>
-      <c r="F129" s="71" t="s">
+      <c r="F129" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="G129" s="72" t="s">
+      <c r="G129" s="66" t="s">
         <v>68</v>
       </c>
       <c r="H129" s="30"/>
@@ -5588,10 +5586,10 @@
       <c r="C130" s="29"/>
       <c r="D130" s="30"/>
       <c r="E130" s="36"/>
-      <c r="F130" s="61" t="s">
+      <c r="F130" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="G130" s="67" t="s">
+      <c r="G130" s="61" t="s">
         <v>66</v>
       </c>
       <c r="H130" s="30"/>
@@ -5621,13 +5619,13 @@
       <c r="C131" s="29"/>
       <c r="D131" s="30"/>
       <c r="E131" s="36"/>
-      <c r="F131" s="61" t="s">
+      <c r="F131" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="G131" s="75" t="s">
+      <c r="G131" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="H131" s="74"/>
+      <c r="H131" s="68"/>
       <c r="I131" s="30"/>
       <c r="J131" s="30"/>
       <c r="K131" s="30"/>
@@ -5653,11 +5651,11 @@
       <c r="B132" s="6"/>
       <c r="C132" s="29"/>
       <c r="D132" s="30"/>
-      <c r="E132" s="59"/>
-      <c r="F132" s="71" t="s">
+      <c r="E132" s="53"/>
+      <c r="F132" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="G132" s="72" t="s">
+      <c r="G132" s="66" t="s">
         <v>71</v>
       </c>
       <c r="H132" s="30"/>
@@ -5686,11 +5684,11 @@
       <c r="B133" s="6"/>
       <c r="C133" s="29"/>
       <c r="D133" s="30"/>
-      <c r="E133" s="59"/>
-      <c r="F133" s="61" t="s">
+      <c r="E133" s="53"/>
+      <c r="F133" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="G133" s="67" t="s">
+      <c r="G133" s="61" t="s">
         <v>72</v>
       </c>
       <c r="H133" s="30"/>
@@ -5718,13 +5716,13 @@
     <row r="134" spans="2:28">
       <c r="B134" s="6"/>
       <c r="C134" s="29"/>
-      <c r="D134" s="62" t="s">
+      <c r="D134" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="E134" s="54" t="s">
+      <c r="E134" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="F134" s="58"/>
+      <c r="F134" s="52"/>
       <c r="G134" s="30"/>
       <c r="H134" s="30"/>
       <c r="I134" s="30"/>
@@ -5752,23 +5750,23 @@
       <c r="B135" s="6"/>
       <c r="C135" s="29"/>
       <c r="D135" s="30"/>
-      <c r="E135" s="73" t="s">
+      <c r="E135" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="F135" s="73"/>
-      <c r="G135" s="74"/>
-      <c r="H135" s="74"/>
-      <c r="I135" s="74"/>
-      <c r="J135" s="74"/>
-      <c r="K135" s="74"/>
-      <c r="L135" s="74"/>
-      <c r="M135" s="74"/>
-      <c r="N135" s="76"/>
+      <c r="F135" s="67"/>
+      <c r="G135" s="68"/>
+      <c r="H135" s="68"/>
+      <c r="I135" s="68"/>
+      <c r="J135" s="68"/>
+      <c r="K135" s="68"/>
+      <c r="L135" s="68"/>
+      <c r="M135" s="68"/>
+      <c r="N135" s="70"/>
       <c r="O135" s="30"/>
-      <c r="P135" s="61" t="s">
+      <c r="P135" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="Q135" s="67" t="s">
+      <c r="Q135" s="61" t="s">
         <v>75</v>
       </c>
       <c r="R135" s="30"/>
@@ -5787,8 +5785,8 @@
       <c r="B136" s="6"/>
       <c r="C136" s="29"/>
       <c r="D136" s="30"/>
-      <c r="E136" s="68"/>
-      <c r="F136" s="68"/>
+      <c r="E136" s="62"/>
+      <c r="F136" s="62"/>
       <c r="G136" s="37"/>
       <c r="H136" s="37"/>
       <c r="I136" s="37"/>
@@ -5798,8 +5796,8 @@
       <c r="M136" s="37"/>
       <c r="N136" s="36"/>
       <c r="O136" s="30"/>
-      <c r="P136" s="61"/>
-      <c r="Q136" s="67"/>
+      <c r="P136" s="55"/>
+      <c r="Q136" s="61"/>
       <c r="R136" s="30"/>
       <c r="S136" s="30"/>
       <c r="T136" s="30"/>
@@ -5816,23 +5814,23 @@
       <c r="B137" s="6"/>
       <c r="C137" s="29"/>
       <c r="D137" s="30"/>
-      <c r="E137" s="73" t="s">
+      <c r="E137" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="F137" s="73"/>
-      <c r="G137" s="74"/>
-      <c r="H137" s="74"/>
-      <c r="I137" s="74"/>
-      <c r="J137" s="74"/>
-      <c r="K137" s="74"/>
-      <c r="L137" s="74"/>
-      <c r="M137" s="74"/>
-      <c r="N137" s="76"/>
+      <c r="F137" s="67"/>
+      <c r="G137" s="68"/>
+      <c r="H137" s="68"/>
+      <c r="I137" s="68"/>
+      <c r="J137" s="68"/>
+      <c r="K137" s="68"/>
+      <c r="L137" s="68"/>
+      <c r="M137" s="68"/>
+      <c r="N137" s="70"/>
       <c r="O137" s="30"/>
-      <c r="P137" s="61" t="s">
+      <c r="P137" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="Q137" s="67" t="s">
+      <c r="Q137" s="61" t="s">
         <v>77</v>
       </c>
       <c r="R137" s="30"/>
@@ -5851,8 +5849,8 @@
       <c r="B138" s="6"/>
       <c r="C138" s="29"/>
       <c r="D138" s="30"/>
-      <c r="E138" s="68"/>
-      <c r="F138" s="68"/>
+      <c r="E138" s="62"/>
+      <c r="F138" s="62"/>
       <c r="G138" s="37"/>
       <c r="H138" s="37"/>
       <c r="I138" s="37"/>
@@ -5862,8 +5860,8 @@
       <c r="M138" s="37"/>
       <c r="N138" s="36"/>
       <c r="O138" s="30"/>
-      <c r="P138" s="61"/>
-      <c r="Q138" s="67"/>
+      <c r="P138" s="55"/>
+      <c r="Q138" s="61"/>
       <c r="R138" s="30"/>
       <c r="S138" s="30"/>
       <c r="T138" s="30"/>
@@ -5880,23 +5878,23 @@
       <c r="B139" s="6"/>
       <c r="C139" s="29"/>
       <c r="D139" s="30"/>
-      <c r="E139" s="73" t="s">
+      <c r="E139" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="F139" s="73"/>
-      <c r="G139" s="74"/>
-      <c r="H139" s="74"/>
-      <c r="I139" s="74"/>
-      <c r="J139" s="74"/>
-      <c r="K139" s="74"/>
-      <c r="L139" s="74"/>
-      <c r="M139" s="74"/>
-      <c r="N139" s="76"/>
+      <c r="F139" s="67"/>
+      <c r="G139" s="68"/>
+      <c r="H139" s="68"/>
+      <c r="I139" s="68"/>
+      <c r="J139" s="68"/>
+      <c r="K139" s="68"/>
+      <c r="L139" s="68"/>
+      <c r="M139" s="68"/>
+      <c r="N139" s="70"/>
       <c r="O139" s="30"/>
-      <c r="P139" s="61" t="s">
+      <c r="P139" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="Q139" s="67" t="s">
+      <c r="Q139" s="61" t="s">
         <v>78</v>
       </c>
       <c r="R139" s="30"/>
@@ -5955,9 +5953,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A48E2B-8799-4E49-8789-1A12BF601F16}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:AC124"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="115" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="15"/>
   <cols>
@@ -5970,100 +5971,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="14.25">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="46"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
+      <c r="AB1" s="74"/>
     </row>
     <row r="2" spans="2:28" ht="14.25">
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="49"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="76"/>
+      <c r="W2" s="76"/>
+      <c r="X2" s="76"/>
+      <c r="Y2" s="76"/>
+      <c r="Z2" s="76"/>
+      <c r="AA2" s="76"/>
+      <c r="AB2" s="77"/>
     </row>
     <row r="3" spans="2:28" ht="14.25">
-      <c r="B3" s="47"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
-      <c r="T3" s="48"/>
-      <c r="U3" s="48"/>
-      <c r="V3" s="48"/>
-      <c r="W3" s="48"/>
-      <c r="X3" s="48"/>
-      <c r="Y3" s="48"/>
-      <c r="Z3" s="48"/>
-      <c r="AA3" s="48"/>
-      <c r="AB3" s="49"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="76"/>
+      <c r="AB3" s="77"/>
     </row>
     <row r="4" spans="2:28" ht="20.100000000000001" customHeight="1">
       <c r="B4" s="4"/>
       <c r="C4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="D4" s="60" t="s">
         <v>56</v>
       </c>
       <c r="E4" s="5"/>
@@ -6091,7 +6092,7 @@
       <c r="AA4" s="5"/>
       <c r="AB4" s="22"/>
     </row>
-    <row r="5" spans="2:28" s="1" customFormat="1">
+    <row r="5" spans="2:28">
       <c r="B5" s="6"/>
       <c r="C5" s="29"/>
       <c r="D5" s="30"/>
@@ -6120,21 +6121,21 @@
       <c r="AA5" s="30"/>
       <c r="AB5" s="35"/>
     </row>
-    <row r="6" spans="2:28" s="1" customFormat="1">
+    <row r="6" spans="2:28">
       <c r="B6" s="6"/>
       <c r="C6" s="29"/>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="77"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
       <c r="I6" s="30"/>
-      <c r="J6" s="61" t="s">
+      <c r="J6" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="67" t="s">
+      <c r="K6" s="61" t="s">
         <v>58</v>
       </c>
       <c r="L6" s="30"/>
@@ -6155,7 +6156,7 @@
       <c r="AA6" s="30"/>
       <c r="AB6" s="35"/>
     </row>
-    <row r="7" spans="2:28" s="1" customFormat="1">
+    <row r="7" spans="2:28">
       <c r="B7" s="6"/>
       <c r="C7" s="29"/>
       <c r="G7" s="30"/>
@@ -6181,21 +6182,21 @@
       <c r="AA7" s="30"/>
       <c r="AB7" s="35"/>
     </row>
-    <row r="8" spans="2:28" s="1" customFormat="1">
+    <row r="8" spans="2:28">
       <c r="B8" s="6"/>
       <c r="C8" s="29"/>
-      <c r="D8" s="73" t="s">
+      <c r="D8" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="77"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
       <c r="I8" s="30"/>
-      <c r="J8" s="61" t="s">
+      <c r="J8" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="67" t="s">
+      <c r="K8" s="61" t="s">
         <v>60</v>
       </c>
       <c r="L8" s="30"/>
@@ -6216,7 +6217,7 @@
       <c r="AA8" s="30"/>
       <c r="AB8" s="35"/>
     </row>
-    <row r="9" spans="2:28" s="1" customFormat="1">
+    <row r="9" spans="2:28">
       <c r="B9" s="6"/>
       <c r="C9" s="29"/>
       <c r="D9" s="30"/>
@@ -6245,7 +6246,7 @@
       <c r="AA9" s="30"/>
       <c r="AB9" s="35"/>
     </row>
-    <row r="10" spans="2:28" s="1" customFormat="1">
+    <row r="10" spans="2:28">
       <c r="B10" s="6"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
@@ -6274,7 +6275,7 @@
       <c r="AA10" s="30"/>
       <c r="AB10" s="35"/>
     </row>
-    <row r="11" spans="2:28" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="2:28" ht="20.100000000000001" customHeight="1">
       <c r="B11" s="4"/>
       <c r="C11" s="42" t="s">
         <v>5</v>
@@ -6307,7 +6308,7 @@
       <c r="AA11" s="5"/>
       <c r="AB11" s="22"/>
     </row>
-    <row r="12" spans="2:28" s="1" customFormat="1">
+    <row r="12" spans="2:28">
       <c r="B12" s="6"/>
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
@@ -6336,7 +6337,7 @@
       <c r="AA12" s="30"/>
       <c r="AB12" s="35"/>
     </row>
-    <row r="13" spans="2:28" s="1" customFormat="1" ht="15.75">
+    <row r="13" spans="2:28" ht="15.75">
       <c r="B13" s="6"/>
       <c r="C13" s="29"/>
       <c r="D13" s="30" t="s">
@@ -6369,7 +6370,7 @@
       <c r="AA13" s="30"/>
       <c r="AB13" s="35"/>
     </row>
-    <row r="14" spans="2:28" s="1" customFormat="1">
+    <row r="14" spans="2:28">
       <c r="B14" s="6"/>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
@@ -6398,7 +6399,7 @@
       <c r="AA14" s="30"/>
       <c r="AB14" s="35"/>
     </row>
-    <row r="15" spans="2:28" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="2:28" ht="20.100000000000001" customHeight="1">
       <c r="B15" s="4"/>
       <c r="C15" s="42" t="s">
         <v>9</v>
@@ -6431,7 +6432,7 @@
       <c r="AA15" s="5"/>
       <c r="AB15" s="22"/>
     </row>
-    <row r="16" spans="2:28" s="1" customFormat="1">
+    <row r="16" spans="2:28">
       <c r="B16" s="6"/>
       <c r="C16" s="29"/>
       <c r="D16" s="30"/>
@@ -6460,7 +6461,7 @@
       <c r="AA16" s="30"/>
       <c r="AB16" s="35"/>
     </row>
-    <row r="17" spans="2:28" s="1" customFormat="1">
+    <row r="17" spans="2:28">
       <c r="B17" s="6"/>
       <c r="C17" s="29"/>
       <c r="D17" s="43" t="s">
@@ -6493,7 +6494,7 @@
       <c r="AA17" s="30"/>
       <c r="AB17" s="35"/>
     </row>
-    <row r="18" spans="2:28" s="1" customFormat="1">
+    <row r="18" spans="2:28">
       <c r="B18" s="6"/>
       <c r="C18" s="29"/>
       <c r="D18" s="32"/>
@@ -6524,14 +6525,14 @@
       <c r="AA18" s="30"/>
       <c r="AB18" s="35"/>
     </row>
-    <row r="19" spans="2:28" s="1" customFormat="1">
+    <row r="19" spans="2:28">
       <c r="B19" s="6"/>
       <c r="C19" s="29"/>
       <c r="D19" s="30"/>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="51" t="s">
+      <c r="F19" s="45" t="s">
         <v>38</v>
       </c>
       <c r="G19" s="15"/>
@@ -6557,11 +6558,11 @@
       <c r="AA19" s="30"/>
       <c r="AB19" s="35"/>
     </row>
-    <row r="20" spans="2:28" s="1" customFormat="1">
+    <row r="20" spans="2:28">
       <c r="B20" s="6"/>
       <c r="C20" s="29"/>
       <c r="D20" s="30"/>
-      <c r="E20" s="53" t="s">
+      <c r="E20" s="47" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="17" t="s">
@@ -6590,11 +6591,11 @@
       <c r="AA20" s="30"/>
       <c r="AB20" s="35"/>
     </row>
-    <row r="21" spans="2:28" s="1" customFormat="1">
+    <row r="21" spans="2:28">
       <c r="B21" s="6"/>
       <c r="C21" s="29"/>
       <c r="D21" s="30"/>
-      <c r="E21" s="53" t="s">
+      <c r="E21" s="47" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="17" t="s">
@@ -6623,7 +6624,7 @@
       <c r="AA21" s="30"/>
       <c r="AB21" s="35"/>
     </row>
-    <row r="22" spans="2:28" s="1" customFormat="1">
+    <row r="22" spans="2:28">
       <c r="B22" s="6"/>
       <c r="C22" s="29"/>
       <c r="D22" s="30"/>
@@ -6652,7 +6653,7 @@
       <c r="AA22" s="30"/>
       <c r="AB22" s="35"/>
     </row>
-    <row r="23" spans="2:28" s="1" customFormat="1">
+    <row r="23" spans="2:28">
       <c r="B23" s="6"/>
       <c r="C23" s="29"/>
       <c r="D23" s="43" t="s">
@@ -6685,7 +6686,7 @@
       <c r="AA23" s="30"/>
       <c r="AB23" s="35"/>
     </row>
-    <row r="24" spans="2:28" s="1" customFormat="1">
+    <row r="24" spans="2:28">
       <c r="B24" s="6"/>
       <c r="C24" s="29"/>
       <c r="D24" s="18"/>
@@ -6716,7 +6717,7 @@
       <c r="AA24" s="30"/>
       <c r="AB24" s="35"/>
     </row>
-    <row r="25" spans="2:28" s="1" customFormat="1">
+    <row r="25" spans="2:28">
       <c r="B25" s="6"/>
       <c r="C25" s="29"/>
       <c r="D25" s="18"/>
@@ -6745,7 +6746,7 @@
       <c r="AA25" s="30"/>
       <c r="AB25" s="35"/>
     </row>
-    <row r="26" spans="2:28" s="1" customFormat="1">
+    <row r="26" spans="2:28">
       <c r="B26" s="6"/>
       <c r="C26" s="29"/>
       <c r="D26" s="18"/>
@@ -6774,7 +6775,7 @@
       <c r="AA26" s="30"/>
       <c r="AB26" s="35"/>
     </row>
-    <row r="27" spans="2:28" s="1" customFormat="1">
+    <row r="27" spans="2:28">
       <c r="B27" s="6"/>
       <c r="C27" s="29"/>
       <c r="D27" s="18"/>
@@ -6803,7 +6804,7 @@
       <c r="AA27" s="30"/>
       <c r="AB27" s="35"/>
     </row>
-    <row r="28" spans="2:28" s="1" customFormat="1">
+    <row r="28" spans="2:28">
       <c r="B28" s="6"/>
       <c r="C28" s="29"/>
       <c r="D28" s="18"/>
@@ -6832,7 +6833,7 @@
       <c r="AA28" s="30"/>
       <c r="AB28" s="35"/>
     </row>
-    <row r="29" spans="2:28" s="1" customFormat="1">
+    <row r="29" spans="2:28">
       <c r="B29" s="6"/>
       <c r="C29" s="29"/>
       <c r="D29" s="18"/>
@@ -6861,7 +6862,7 @@
       <c r="AA29" s="30"/>
       <c r="AB29" s="35"/>
     </row>
-    <row r="30" spans="2:28" s="1" customFormat="1">
+    <row r="30" spans="2:28">
       <c r="B30" s="6"/>
       <c r="C30" s="29"/>
       <c r="D30" s="18"/>
@@ -6890,7 +6891,7 @@
       <c r="AA30" s="30"/>
       <c r="AB30" s="35"/>
     </row>
-    <row r="31" spans="2:28" s="1" customFormat="1">
+    <row r="31" spans="2:28">
       <c r="B31" s="6"/>
       <c r="C31" s="29"/>
       <c r="D31" s="18"/>
@@ -6919,7 +6920,7 @@
       <c r="AA31" s="30"/>
       <c r="AB31" s="35"/>
     </row>
-    <row r="32" spans="2:28" s="1" customFormat="1">
+    <row r="32" spans="2:28">
       <c r="B32" s="6"/>
       <c r="C32" s="29"/>
       <c r="D32" s="18"/>
@@ -6948,7 +6949,7 @@
       <c r="AA32" s="30"/>
       <c r="AB32" s="35"/>
     </row>
-    <row r="33" spans="2:28" s="1" customFormat="1">
+    <row r="33" spans="2:28">
       <c r="B33" s="6"/>
       <c r="C33" s="29"/>
       <c r="D33" s="18"/>
@@ -6977,7 +6978,7 @@
       <c r="AA33" s="30"/>
       <c r="AB33" s="35"/>
     </row>
-    <row r="34" spans="2:28" s="1" customFormat="1">
+    <row r="34" spans="2:28">
       <c r="B34" s="6"/>
       <c r="C34" s="29"/>
       <c r="D34" s="18"/>
@@ -7006,7 +7007,7 @@
       <c r="AA34" s="30"/>
       <c r="AB34" s="35"/>
     </row>
-    <row r="35" spans="2:28" s="1" customFormat="1">
+    <row r="35" spans="2:28">
       <c r="B35" s="6"/>
       <c r="C35" s="29"/>
       <c r="D35" s="18"/>
@@ -7035,7 +7036,7 @@
       <c r="AA35" s="30"/>
       <c r="AB35" s="35"/>
     </row>
-    <row r="36" spans="2:28" s="1" customFormat="1">
+    <row r="36" spans="2:28">
       <c r="B36" s="6"/>
       <c r="C36" s="29"/>
       <c r="D36" s="18"/>
@@ -7064,7 +7065,7 @@
       <c r="AA36" s="30"/>
       <c r="AB36" s="35"/>
     </row>
-    <row r="37" spans="2:28" s="1" customFormat="1">
+    <row r="37" spans="2:28">
       <c r="B37" s="6"/>
       <c r="C37" s="29"/>
       <c r="D37" s="18"/>
@@ -7093,7 +7094,7 @@
       <c r="AA37" s="30"/>
       <c r="AB37" s="35"/>
     </row>
-    <row r="38" spans="2:28" s="1" customFormat="1">
+    <row r="38" spans="2:28">
       <c r="B38" s="6"/>
       <c r="C38" s="29"/>
       <c r="D38" s="20"/>
@@ -7122,7 +7123,7 @@
       <c r="AA38" s="30"/>
       <c r="AB38" s="35"/>
     </row>
-    <row r="39" spans="2:28" s="1" customFormat="1">
+    <row r="39" spans="2:28">
       <c r="B39" s="6"/>
       <c r="C39" s="29"/>
       <c r="D39" s="18"/>
@@ -7153,7 +7154,7 @@
       <c r="AA39" s="30"/>
       <c r="AB39" s="35"/>
     </row>
-    <row r="40" spans="2:28" s="1" customFormat="1">
+    <row r="40" spans="2:28">
       <c r="B40" s="6"/>
       <c r="C40" s="29"/>
       <c r="D40" s="18"/>
@@ -7182,7 +7183,7 @@
       <c r="AA40" s="30"/>
       <c r="AB40" s="35"/>
     </row>
-    <row r="41" spans="2:28" s="1" customFormat="1">
+    <row r="41" spans="2:28">
       <c r="B41" s="6"/>
       <c r="C41" s="29"/>
       <c r="D41" s="18"/>
@@ -7211,7 +7212,7 @@
       <c r="AA41" s="30"/>
       <c r="AB41" s="35"/>
     </row>
-    <row r="42" spans="2:28" s="1" customFormat="1">
+    <row r="42" spans="2:28">
       <c r="B42" s="6"/>
       <c r="C42" s="29"/>
       <c r="D42" s="18"/>
@@ -7240,7 +7241,7 @@
       <c r="AA42" s="30"/>
       <c r="AB42" s="35"/>
     </row>
-    <row r="43" spans="2:28" s="1" customFormat="1">
+    <row r="43" spans="2:28">
       <c r="B43" s="6"/>
       <c r="C43" s="29"/>
       <c r="D43" s="18"/>
@@ -7269,7 +7270,7 @@
       <c r="AA43" s="30"/>
       <c r="AB43" s="35"/>
     </row>
-    <row r="44" spans="2:28" s="1" customFormat="1">
+    <row r="44" spans="2:28">
       <c r="B44" s="6"/>
       <c r="C44" s="29"/>
       <c r="D44" s="18"/>
@@ -7298,7 +7299,7 @@
       <c r="AA44" s="30"/>
       <c r="AB44" s="35"/>
     </row>
-    <row r="45" spans="2:28" s="1" customFormat="1">
+    <row r="45" spans="2:28">
       <c r="B45" s="6"/>
       <c r="C45" s="29"/>
       <c r="D45" s="18"/>
@@ -7327,7 +7328,7 @@
       <c r="AA45" s="30"/>
       <c r="AB45" s="35"/>
     </row>
-    <row r="46" spans="2:28" s="1" customFormat="1">
+    <row r="46" spans="2:28">
       <c r="B46" s="6"/>
       <c r="C46" s="29"/>
       <c r="D46" s="18"/>
@@ -7356,7 +7357,7 @@
       <c r="AA46" s="30"/>
       <c r="AB46" s="35"/>
     </row>
-    <row r="47" spans="2:28" s="1" customFormat="1">
+    <row r="47" spans="2:28">
       <c r="B47" s="6"/>
       <c r="C47" s="29"/>
       <c r="D47" s="18"/>
@@ -7385,7 +7386,7 @@
       <c r="AA47" s="30"/>
       <c r="AB47" s="35"/>
     </row>
-    <row r="48" spans="2:28" s="1" customFormat="1">
+    <row r="48" spans="2:28">
       <c r="B48" s="6"/>
       <c r="C48" s="29"/>
       <c r="D48" s="18"/>
@@ -7414,7 +7415,7 @@
       <c r="AA48" s="30"/>
       <c r="AB48" s="35"/>
     </row>
-    <row r="49" spans="2:28" s="1" customFormat="1">
+    <row r="49" spans="2:28">
       <c r="B49" s="6"/>
       <c r="C49" s="29"/>
       <c r="D49" s="18"/>
@@ -7443,7 +7444,7 @@
       <c r="AA49" s="30"/>
       <c r="AB49" s="35"/>
     </row>
-    <row r="50" spans="2:28" s="1" customFormat="1">
+    <row r="50" spans="2:28">
       <c r="B50" s="6"/>
       <c r="C50" s="29"/>
       <c r="D50" s="18"/>
@@ -7472,7 +7473,7 @@
       <c r="AA50" s="30"/>
       <c r="AB50" s="35"/>
     </row>
-    <row r="51" spans="2:28" s="1" customFormat="1">
+    <row r="51" spans="2:28">
       <c r="B51" s="6"/>
       <c r="C51" s="29"/>
       <c r="D51" s="18"/>
@@ -7501,7 +7502,7 @@
       <c r="AA51" s="30"/>
       <c r="AB51" s="35"/>
     </row>
-    <row r="52" spans="2:28" s="1" customFormat="1">
+    <row r="52" spans="2:28">
       <c r="B52" s="6"/>
       <c r="C52" s="29"/>
       <c r="D52" s="20"/>
@@ -7530,7 +7531,7 @@
       <c r="AA52" s="30"/>
       <c r="AB52" s="35"/>
     </row>
-    <row r="53" spans="2:28" s="1" customFormat="1">
+    <row r="53" spans="2:28">
       <c r="B53" s="6"/>
       <c r="C53" s="29"/>
       <c r="D53" s="18"/>
@@ -7561,7 +7562,7 @@
       <c r="AA53" s="30"/>
       <c r="AB53" s="35"/>
     </row>
-    <row r="54" spans="2:28" s="1" customFormat="1">
+    <row r="54" spans="2:28">
       <c r="B54" s="6"/>
       <c r="C54" s="29"/>
       <c r="D54" s="18"/>
@@ -7590,7 +7591,7 @@
       <c r="AA54" s="30"/>
       <c r="AB54" s="35"/>
     </row>
-    <row r="55" spans="2:28" s="1" customFormat="1">
+    <row r="55" spans="2:28">
       <c r="B55" s="6"/>
       <c r="C55" s="29"/>
       <c r="D55" s="18"/>
@@ -7619,7 +7620,7 @@
       <c r="AA55" s="30"/>
       <c r="AB55" s="35"/>
     </row>
-    <row r="56" spans="2:28" s="1" customFormat="1">
+    <row r="56" spans="2:28">
       <c r="B56" s="6"/>
       <c r="C56" s="29"/>
       <c r="D56" s="18"/>
@@ -7648,7 +7649,7 @@
       <c r="AA56" s="30"/>
       <c r="AB56" s="35"/>
     </row>
-    <row r="57" spans="2:28" s="1" customFormat="1">
+    <row r="57" spans="2:28">
       <c r="B57" s="6"/>
       <c r="C57" s="29"/>
       <c r="D57" s="18"/>
@@ -7677,7 +7678,7 @@
       <c r="AA57" s="30"/>
       <c r="AB57" s="35"/>
     </row>
-    <row r="58" spans="2:28" s="1" customFormat="1">
+    <row r="58" spans="2:28">
       <c r="B58" s="6"/>
       <c r="C58" s="29"/>
       <c r="D58" s="18"/>
@@ -7706,7 +7707,7 @@
       <c r="AA58" s="30"/>
       <c r="AB58" s="35"/>
     </row>
-    <row r="59" spans="2:28" s="1" customFormat="1">
+    <row r="59" spans="2:28">
       <c r="B59" s="6"/>
       <c r="C59" s="29"/>
       <c r="D59" s="18"/>
@@ -7735,7 +7736,7 @@
       <c r="AA59" s="30"/>
       <c r="AB59" s="35"/>
     </row>
-    <row r="60" spans="2:28" s="1" customFormat="1">
+    <row r="60" spans="2:28">
       <c r="B60" s="6"/>
       <c r="C60" s="29"/>
       <c r="D60" s="18"/>
@@ -7764,7 +7765,7 @@
       <c r="AA60" s="30"/>
       <c r="AB60" s="35"/>
     </row>
-    <row r="61" spans="2:28" s="1" customFormat="1">
+    <row r="61" spans="2:28">
       <c r="B61" s="6"/>
       <c r="C61" s="29"/>
       <c r="D61" s="18"/>
@@ -7793,7 +7794,7 @@
       <c r="AA61" s="30"/>
       <c r="AB61" s="35"/>
     </row>
-    <row r="62" spans="2:28" s="1" customFormat="1">
+    <row r="62" spans="2:28">
       <c r="B62" s="6"/>
       <c r="C62" s="29"/>
       <c r="D62" s="18"/>
@@ -7822,7 +7823,7 @@
       <c r="AA62" s="30"/>
       <c r="AB62" s="35"/>
     </row>
-    <row r="63" spans="2:28" s="1" customFormat="1">
+    <row r="63" spans="2:28">
       <c r="B63" s="6"/>
       <c r="C63" s="29"/>
       <c r="D63" s="18"/>
@@ -7851,7 +7852,7 @@
       <c r="AA63" s="30"/>
       <c r="AB63" s="35"/>
     </row>
-    <row r="64" spans="2:28" s="1" customFormat="1">
+    <row r="64" spans="2:28">
       <c r="B64" s="6"/>
       <c r="C64" s="29"/>
       <c r="D64" s="18"/>
@@ -7880,7 +7881,7 @@
       <c r="AA64" s="30"/>
       <c r="AB64" s="35"/>
     </row>
-    <row r="65" spans="2:28" s="1" customFormat="1">
+    <row r="65" spans="2:28">
       <c r="B65" s="6"/>
       <c r="C65" s="29"/>
       <c r="D65" s="18"/>
@@ -7909,7 +7910,7 @@
       <c r="AA65" s="30"/>
       <c r="AB65" s="35"/>
     </row>
-    <row r="66" spans="2:28" s="1" customFormat="1">
+    <row r="66" spans="2:28">
       <c r="B66" s="6"/>
       <c r="C66" s="29"/>
       <c r="D66" s="18"/>
@@ -7938,7 +7939,7 @@
       <c r="AA66" s="30"/>
       <c r="AB66" s="35"/>
     </row>
-    <row r="67" spans="2:28" s="1" customFormat="1">
+    <row r="67" spans="2:28">
       <c r="B67" s="6"/>
       <c r="C67" s="29"/>
       <c r="D67" s="18"/>
@@ -7967,7 +7968,7 @@
       <c r="AA67" s="30"/>
       <c r="AB67" s="35"/>
     </row>
-    <row r="68" spans="2:28" s="1" customFormat="1">
+    <row r="68" spans="2:28">
       <c r="B68" s="6"/>
       <c r="C68" s="29"/>
       <c r="D68" s="18"/>
@@ -7996,7 +7997,7 @@
       <c r="AA68" s="30"/>
       <c r="AB68" s="35"/>
     </row>
-    <row r="69" spans="2:28" s="1" customFormat="1">
+    <row r="69" spans="2:28">
       <c r="B69" s="6"/>
       <c r="C69" s="29"/>
       <c r="D69" s="18"/>
@@ -8025,7 +8026,7 @@
       <c r="AA69" s="30"/>
       <c r="AB69" s="35"/>
     </row>
-    <row r="70" spans="2:28" s="1" customFormat="1">
+    <row r="70" spans="2:28">
       <c r="B70" s="6"/>
       <c r="C70" s="29"/>
       <c r="D70" s="18"/>
@@ -8054,7 +8055,7 @@
       <c r="AA70" s="30"/>
       <c r="AB70" s="35"/>
     </row>
-    <row r="71" spans="2:28" s="1" customFormat="1">
+    <row r="71" spans="2:28">
       <c r="B71" s="6"/>
       <c r="C71" s="29"/>
       <c r="D71" s="18"/>
@@ -8083,7 +8084,7 @@
       <c r="AA71" s="30"/>
       <c r="AB71" s="35"/>
     </row>
-    <row r="72" spans="2:28" s="1" customFormat="1">
+    <row r="72" spans="2:28">
       <c r="B72" s="6"/>
       <c r="C72" s="29"/>
       <c r="D72" s="18"/>
@@ -8112,7 +8113,7 @@
       <c r="AA72" s="30"/>
       <c r="AB72" s="35"/>
     </row>
-    <row r="73" spans="2:28" s="1" customFormat="1">
+    <row r="73" spans="2:28">
       <c r="B73" s="6"/>
       <c r="C73" s="29"/>
       <c r="D73" s="18"/>
@@ -8141,7 +8142,7 @@
       <c r="AA73" s="30"/>
       <c r="AB73" s="35"/>
     </row>
-    <row r="74" spans="2:28" s="1" customFormat="1">
+    <row r="74" spans="2:28">
       <c r="B74" s="6"/>
       <c r="C74" s="29"/>
       <c r="D74" s="20"/>
@@ -8170,7 +8171,7 @@
       <c r="AA74" s="30"/>
       <c r="AB74" s="35"/>
     </row>
-    <row r="75" spans="2:28" s="1" customFormat="1">
+    <row r="75" spans="2:28">
       <c r="B75" s="6"/>
       <c r="C75" s="29"/>
       <c r="D75" s="32"/>
@@ -8199,7 +8200,7 @@
       <c r="AA75" s="30"/>
       <c r="AB75" s="35"/>
     </row>
-    <row r="76" spans="2:28" s="1" customFormat="1">
+    <row r="76" spans="2:28">
       <c r="B76" s="6"/>
       <c r="C76" s="29"/>
       <c r="D76" s="30"/>
@@ -8228,12 +8229,12 @@
       <c r="AA76" s="30"/>
       <c r="AB76" s="35"/>
     </row>
-    <row r="77" spans="2:28" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="77" spans="2:28" ht="20.100000000000001" customHeight="1">
       <c r="B77" s="4"/>
       <c r="C77" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D77" s="66" t="s">
+      <c r="D77" s="60" t="s">
         <v>55</v>
       </c>
       <c r="E77" s="5"/>
@@ -8261,7 +8262,7 @@
       <c r="AA77" s="5"/>
       <c r="AB77" s="22"/>
     </row>
-    <row r="78" spans="2:28" s="1" customFormat="1">
+    <row r="78" spans="2:28">
       <c r="B78" s="6"/>
       <c r="C78" s="29"/>
       <c r="D78" s="30"/>
@@ -8290,7 +8291,7 @@
       <c r="AA78" s="30"/>
       <c r="AB78" s="35"/>
     </row>
-    <row r="79" spans="2:28" s="1" customFormat="1">
+    <row r="79" spans="2:28">
       <c r="B79" s="6"/>
       <c r="C79" s="29"/>
       <c r="D79" s="43" t="s">
@@ -8323,11 +8324,11 @@
       <c r="AA79" s="30"/>
       <c r="AB79" s="35"/>
     </row>
-    <row r="80" spans="2:28" s="1" customFormat="1">
+    <row r="80" spans="2:28">
       <c r="B80" s="6"/>
       <c r="C80" s="29"/>
       <c r="D80" s="30"/>
-      <c r="E80" s="50" t="s">
+      <c r="E80" s="44" t="s">
         <v>3</v>
       </c>
       <c r="F80" s="24" t="s">
@@ -8356,7 +8357,7 @@
       <c r="AA80" s="30"/>
       <c r="AB80" s="35"/>
     </row>
-    <row r="81" spans="2:28" s="1" customFormat="1">
+    <row r="81" spans="2:28">
       <c r="B81" s="6"/>
       <c r="C81" s="29"/>
       <c r="D81" s="30"/>
@@ -8389,7 +8390,7 @@
       <c r="AA81" s="30"/>
       <c r="AB81" s="35"/>
     </row>
-    <row r="82" spans="2:28" s="1" customFormat="1">
+    <row r="82" spans="2:28">
       <c r="B82" s="6"/>
       <c r="C82" s="29"/>
       <c r="D82" s="30"/>
@@ -8422,7 +8423,7 @@
       <c r="AA82" s="30"/>
       <c r="AB82" s="35"/>
     </row>
-    <row r="83" spans="2:28" s="1" customFormat="1">
+    <row r="83" spans="2:28">
       <c r="B83" s="6"/>
       <c r="C83" s="29"/>
       <c r="D83" s="30"/>
@@ -8455,11 +8456,11 @@
       <c r="AA83" s="30"/>
       <c r="AB83" s="35"/>
     </row>
-    <row r="84" spans="2:28" s="1" customFormat="1">
+    <row r="84" spans="2:28">
       <c r="B84" s="6"/>
       <c r="C84" s="29"/>
       <c r="D84" s="30"/>
-      <c r="E84" s="50" t="s">
+      <c r="E84" s="44" t="s">
         <v>3</v>
       </c>
       <c r="F84" s="24" t="s">
@@ -8488,11 +8489,11 @@
       <c r="AA84" s="30"/>
       <c r="AB84" s="35"/>
     </row>
-    <row r="85" spans="2:28" s="1" customFormat="1">
+    <row r="85" spans="2:28">
       <c r="B85" s="6"/>
       <c r="C85" s="29"/>
       <c r="D85" s="32"/>
-      <c r="E85" s="50" t="s">
+      <c r="E85" s="44" t="s">
         <v>3</v>
       </c>
       <c r="F85" s="24" t="s">
@@ -8521,11 +8522,11 @@
       <c r="AA85" s="30"/>
       <c r="AB85" s="35"/>
     </row>
-    <row r="86" spans="2:28" s="1" customFormat="1">
+    <row r="86" spans="2:28">
       <c r="B86" s="6"/>
       <c r="C86" s="29"/>
       <c r="D86" s="30"/>
-      <c r="E86" s="50" t="s">
+      <c r="E86" s="44" t="s">
         <v>3</v>
       </c>
       <c r="F86" s="24" t="s">
@@ -8554,7 +8555,7 @@
       <c r="AA86" s="30"/>
       <c r="AB86" s="35"/>
     </row>
-    <row r="87" spans="2:28" s="1" customFormat="1">
+    <row r="87" spans="2:28">
       <c r="B87" s="6"/>
       <c r="C87" s="29"/>
       <c r="D87" s="30"/>
@@ -8587,7 +8588,7 @@
       <c r="AA87" s="30"/>
       <c r="AB87" s="35"/>
     </row>
-    <row r="88" spans="2:28" s="1" customFormat="1">
+    <row r="88" spans="2:28">
       <c r="B88" s="6"/>
       <c r="C88" s="29"/>
       <c r="D88" s="30"/>
@@ -8616,13 +8617,13 @@
       <c r="AA88" s="30"/>
       <c r="AB88" s="35"/>
     </row>
-    <row r="89" spans="2:28" s="1" customFormat="1">
+    <row r="89" spans="2:28">
       <c r="B89" s="6"/>
       <c r="C89" s="29"/>
       <c r="D89" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="E89" s="54" t="s">
+      <c r="E89" s="48" t="s">
         <v>39</v>
       </c>
       <c r="F89" s="30"/>
@@ -8649,14 +8650,14 @@
       <c r="AA89" s="30"/>
       <c r="AB89" s="35"/>
     </row>
-    <row r="90" spans="2:28" s="1" customFormat="1">
+    <row r="90" spans="2:28">
       <c r="B90" s="6"/>
       <c r="C90" s="29"/>
       <c r="D90" s="30"/>
-      <c r="E90" s="59" t="s">
+      <c r="E90" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F90" s="58" t="s">
+      <c r="F90" s="52" t="s">
         <v>40</v>
       </c>
       <c r="G90" s="30"/>
@@ -8682,14 +8683,14 @@
       <c r="AA90" s="30"/>
       <c r="AB90" s="35"/>
     </row>
-    <row r="91" spans="2:28" s="1" customFormat="1">
+    <row r="91" spans="2:28">
       <c r="B91" s="6"/>
       <c r="C91" s="29"/>
       <c r="D91" s="30"/>
       <c r="E91" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F91" s="60" t="s">
+      <c r="F91" s="54" t="s">
         <v>41</v>
       </c>
       <c r="G91" s="30"/>
@@ -8715,80 +8716,80 @@
       <c r="AA91" s="30"/>
       <c r="AB91" s="35"/>
     </row>
-    <row r="92" spans="2:28" s="1" customFormat="1">
+    <row r="92" spans="2:28">
       <c r="B92" s="6"/>
       <c r="C92" s="29"/>
       <c r="D92" s="30"/>
-      <c r="E92" s="59" t="s">
+      <c r="E92" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F92" s="58" t="s">
+      <c r="F92" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="G92" s="56"/>
-      <c r="H92" s="57"/>
-      <c r="I92" s="57"/>
-      <c r="J92" s="57"/>
-      <c r="K92" s="57"/>
-      <c r="L92" s="57"/>
-      <c r="M92" s="57"/>
-      <c r="N92" s="57"/>
-      <c r="O92" s="57"/>
-      <c r="P92" s="57"/>
-      <c r="Q92" s="57"/>
-      <c r="R92" s="57"/>
-      <c r="S92" s="57"/>
-      <c r="T92" s="57"/>
-      <c r="U92" s="57"/>
-      <c r="V92" s="57"/>
-      <c r="W92" s="57"/>
-      <c r="X92" s="57"/>
+      <c r="G92" s="50"/>
+      <c r="H92" s="51"/>
+      <c r="I92" s="51"/>
+      <c r="J92" s="51"/>
+      <c r="K92" s="51"/>
+      <c r="L92" s="51"/>
+      <c r="M92" s="51"/>
+      <c r="N92" s="51"/>
+      <c r="O92" s="51"/>
+      <c r="P92" s="51"/>
+      <c r="Q92" s="51"/>
+      <c r="R92" s="51"/>
+      <c r="S92" s="51"/>
+      <c r="T92" s="51"/>
+      <c r="U92" s="51"/>
+      <c r="V92" s="51"/>
+      <c r="W92" s="51"/>
+      <c r="X92" s="51"/>
       <c r="Y92" s="30"/>
       <c r="Z92" s="30"/>
       <c r="AA92" s="30"/>
       <c r="AB92" s="35"/>
     </row>
-    <row r="93" spans="2:28" s="1" customFormat="1">
+    <row r="93" spans="2:28">
       <c r="B93" s="6"/>
       <c r="C93" s="29"/>
       <c r="D93" s="30"/>
-      <c r="E93" s="61" t="s">
+      <c r="E93" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="F93" s="60" t="s">
+      <c r="F93" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G93" s="56"/>
-      <c r="H93" s="57"/>
-      <c r="I93" s="57"/>
-      <c r="J93" s="57"/>
-      <c r="K93" s="57"/>
-      <c r="L93" s="57"/>
-      <c r="M93" s="57"/>
-      <c r="N93" s="57"/>
-      <c r="O93" s="57"/>
-      <c r="P93" s="57"/>
-      <c r="Q93" s="57"/>
-      <c r="R93" s="57"/>
-      <c r="S93" s="57"/>
-      <c r="T93" s="57"/>
-      <c r="U93" s="57"/>
-      <c r="V93" s="57"/>
-      <c r="W93" s="57"/>
-      <c r="X93" s="57"/>
+      <c r="G93" s="50"/>
+      <c r="H93" s="51"/>
+      <c r="I93" s="51"/>
+      <c r="J93" s="51"/>
+      <c r="K93" s="51"/>
+      <c r="L93" s="51"/>
+      <c r="M93" s="51"/>
+      <c r="N93" s="51"/>
+      <c r="O93" s="51"/>
+      <c r="P93" s="51"/>
+      <c r="Q93" s="51"/>
+      <c r="R93" s="51"/>
+      <c r="S93" s="51"/>
+      <c r="T93" s="51"/>
+      <c r="U93" s="51"/>
+      <c r="V93" s="51"/>
+      <c r="W93" s="51"/>
+      <c r="X93" s="51"/>
       <c r="Y93" s="30"/>
       <c r="Z93" s="30"/>
       <c r="AA93" s="30"/>
       <c r="AB93" s="35"/>
     </row>
-    <row r="94" spans="2:28" s="1" customFormat="1">
+    <row r="94" spans="2:28">
       <c r="B94" s="6"/>
       <c r="C94" s="29"/>
       <c r="D94" s="30"/>
-      <c r="E94" s="59" t="s">
+      <c r="E94" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F94" s="58" t="s">
+      <c r="F94" s="52" t="s">
         <v>44</v>
       </c>
       <c r="G94" s="30"/>
@@ -8814,14 +8815,14 @@
       <c r="AA94" s="30"/>
       <c r="AB94" s="35"/>
     </row>
-    <row r="95" spans="2:28" s="1" customFormat="1">
+    <row r="95" spans="2:28">
       <c r="B95" s="6"/>
       <c r="C95" s="29"/>
       <c r="D95" s="30"/>
-      <c r="E95" s="61" t="s">
+      <c r="E95" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="F95" s="60" t="s">
+      <c r="F95" s="54" t="s">
         <v>45</v>
       </c>
       <c r="G95" s="30"/>
@@ -8847,7 +8848,7 @@
       <c r="AA95" s="30"/>
       <c r="AB95" s="35"/>
     </row>
-    <row r="96" spans="2:28" s="1" customFormat="1">
+    <row r="96" spans="2:28">
       <c r="B96" s="6"/>
       <c r="C96" s="29"/>
       <c r="D96" s="30"/>
@@ -8876,7 +8877,7 @@
       <c r="AA96" s="30"/>
       <c r="AB96" s="35"/>
     </row>
-    <row r="97" spans="2:28" s="1" customFormat="1">
+    <row r="97" spans="2:28">
       <c r="B97" s="6"/>
       <c r="C97" s="29"/>
       <c r="D97"/>
@@ -8905,12 +8906,12 @@
       <c r="AA97" s="30"/>
       <c r="AB97" s="35"/>
     </row>
-    <row r="98" spans="2:28" s="1" customFormat="1">
+    <row r="98" spans="2:28">
       <c r="B98" s="6"/>
       <c r="C98" s="29"/>
       <c r="D98" s="30"/>
       <c r="E98" s="30"/>
-      <c r="F98" s="55"/>
+      <c r="F98" s="49"/>
       <c r="G98" s="30"/>
       <c r="H98" s="30"/>
       <c r="I98" s="30"/>
@@ -8934,7 +8935,7 @@
       <c r="AA98" s="30"/>
       <c r="AB98" s="35"/>
     </row>
-    <row r="99" spans="2:28" s="1" customFormat="1">
+    <row r="99" spans="2:28">
       <c r="B99" s="6"/>
       <c r="C99" s="29"/>
       <c r="D99" s="30"/>
@@ -8963,7 +8964,7 @@
       <c r="AA99" s="30"/>
       <c r="AB99" s="35"/>
     </row>
-    <row r="100" spans="2:28" s="1" customFormat="1">
+    <row r="100" spans="2:28">
       <c r="B100" s="6"/>
       <c r="C100" s="29"/>
       <c r="D100" s="30"/>
@@ -8992,12 +8993,12 @@
       <c r="AA100" s="30"/>
       <c r="AB100" s="35"/>
     </row>
-    <row r="101" spans="2:28" s="1" customFormat="1">
+    <row r="101" spans="2:28">
       <c r="B101" s="6"/>
       <c r="C101" s="29"/>
       <c r="D101" s="30"/>
       <c r="E101" s="30"/>
-      <c r="F101" s="55"/>
+      <c r="F101" s="49"/>
       <c r="G101" s="30"/>
       <c r="H101" s="30"/>
       <c r="I101" s="30"/>
@@ -9021,7 +9022,7 @@
       <c r="AA101" s="30"/>
       <c r="AB101" s="35"/>
     </row>
-    <row r="102" spans="2:28" s="1" customFormat="1">
+    <row r="102" spans="2:28">
       <c r="B102" s="6"/>
       <c r="C102" s="29"/>
       <c r="D102" s="30"/>
@@ -9050,7 +9051,7 @@
       <c r="AA102" s="30"/>
       <c r="AB102" s="35"/>
     </row>
-    <row r="103" spans="2:28" s="1" customFormat="1">
+    <row r="103" spans="2:28">
       <c r="B103" s="6"/>
       <c r="C103" s="29"/>
       <c r="D103" s="30"/>
@@ -9079,12 +9080,12 @@
       <c r="AA103" s="30"/>
       <c r="AB103" s="35"/>
     </row>
-    <row r="104" spans="2:28" s="1" customFormat="1">
+    <row r="104" spans="2:28">
       <c r="B104" s="6"/>
       <c r="C104" s="29"/>
       <c r="D104" s="30"/>
       <c r="E104" s="30"/>
-      <c r="F104" s="55"/>
+      <c r="F104" s="49"/>
       <c r="G104" s="30"/>
       <c r="H104" s="30"/>
       <c r="I104" s="30"/>
@@ -9108,7 +9109,7 @@
       <c r="AA104" s="30"/>
       <c r="AB104" s="35"/>
     </row>
-    <row r="105" spans="2:28" s="1" customFormat="1">
+    <row r="105" spans="2:28">
       <c r="B105" s="6"/>
       <c r="C105" s="29"/>
       <c r="D105" s="30"/>
@@ -9137,7 +9138,7 @@
       <c r="AA105" s="30"/>
       <c r="AB105" s="35"/>
     </row>
-    <row r="106" spans="2:28" s="1" customFormat="1">
+    <row r="106" spans="2:28">
       <c r="B106" s="6"/>
       <c r="C106" s="29"/>
       <c r="D106" s="30"/>
@@ -9166,12 +9167,12 @@
       <c r="AA106" s="30"/>
       <c r="AB106" s="35"/>
     </row>
-    <row r="107" spans="2:28" s="1" customFormat="1">
+    <row r="107" spans="2:28">
       <c r="B107" s="6"/>
       <c r="C107" s="29"/>
       <c r="D107" s="30"/>
       <c r="E107" s="30"/>
-      <c r="F107" s="55"/>
+      <c r="F107" s="49"/>
       <c r="G107" s="30"/>
       <c r="H107" s="30"/>
       <c r="I107" s="30"/>
@@ -9195,7 +9196,7 @@
       <c r="AA107" s="30"/>
       <c r="AB107" s="35"/>
     </row>
-    <row r="108" spans="2:28" s="1" customFormat="1">
+    <row r="108" spans="2:28">
       <c r="B108" s="6"/>
       <c r="C108" s="29"/>
       <c r="D108" s="30"/>
@@ -9224,7 +9225,7 @@
       <c r="AA108" s="30"/>
       <c r="AB108" s="35"/>
     </row>
-    <row r="109" spans="2:28" s="1" customFormat="1">
+    <row r="109" spans="2:28">
       <c r="B109" s="6"/>
       <c r="C109" s="29"/>
       <c r="D109" s="30"/>
@@ -9253,12 +9254,12 @@
       <c r="AA109" s="30"/>
       <c r="AB109" s="35"/>
     </row>
-    <row r="110" spans="2:28" s="1" customFormat="1">
+    <row r="110" spans="2:28">
       <c r="B110" s="6"/>
       <c r="C110" s="29"/>
       <c r="D110" s="30"/>
       <c r="E110" s="30"/>
-      <c r="F110" s="55"/>
+      <c r="F110" s="49"/>
       <c r="G110" s="30"/>
       <c r="H110" s="30"/>
       <c r="I110" s="30"/>
@@ -9282,7 +9283,7 @@
       <c r="AA110" s="30"/>
       <c r="AB110" s="35"/>
     </row>
-    <row r="111" spans="2:28" s="1" customFormat="1">
+    <row r="111" spans="2:28">
       <c r="B111" s="6"/>
       <c r="C111" s="29"/>
       <c r="D111" s="30"/>
@@ -9311,13 +9312,13 @@
       <c r="AA111" s="30"/>
       <c r="AB111" s="35"/>
     </row>
-    <row r="112" spans="2:28" s="1" customFormat="1">
+    <row r="112" spans="2:28">
       <c r="B112" s="6"/>
       <c r="C112" s="29"/>
-      <c r="D112" s="62" t="s">
+      <c r="D112" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="E112" s="54" t="s">
+      <c r="E112" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F112" s="30"/>
@@ -9344,14 +9345,14 @@
       <c r="AA112" s="30"/>
       <c r="AB112" s="35"/>
     </row>
-    <row r="113" spans="2:28" s="1" customFormat="1">
+    <row r="113" spans="2:28">
       <c r="B113" s="6"/>
       <c r="C113" s="29"/>
       <c r="D113" s="30"/>
-      <c r="E113" s="59" t="s">
+      <c r="E113" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F113" s="58" t="s">
+      <c r="F113" s="52" t="s">
         <v>47</v>
       </c>
       <c r="G113" s="28"/>
@@ -9377,20 +9378,20 @@
       <c r="AA113" s="30"/>
       <c r="AB113" s="35"/>
     </row>
-    <row r="114" spans="2:28" s="1" customFormat="1">
+    <row r="114" spans="2:28">
       <c r="B114" s="6"/>
       <c r="C114" s="29"/>
       <c r="D114" s="30"/>
-      <c r="E114" s="61" t="s">
+      <c r="E114" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="F114" s="65" t="s">
+      <c r="F114" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="G114" s="63"/>
-      <c r="H114" s="64"/>
-      <c r="I114" s="64"/>
-      <c r="J114" s="64"/>
+      <c r="G114" s="57"/>
+      <c r="H114" s="58"/>
+      <c r="I114" s="58"/>
+      <c r="J114" s="58"/>
       <c r="K114" s="30"/>
       <c r="L114" s="30"/>
       <c r="M114" s="30"/>
@@ -9410,14 +9411,14 @@
       <c r="AA114" s="30"/>
       <c r="AB114" s="35"/>
     </row>
-    <row r="115" spans="2:28" s="1" customFormat="1">
+    <row r="115" spans="2:28">
       <c r="B115" s="6"/>
       <c r="C115" s="29"/>
       <c r="D115" s="30"/>
-      <c r="E115" s="59" t="s">
+      <c r="E115" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F115" s="58" t="s">
+      <c r="F115" s="52" t="s">
         <v>49</v>
       </c>
       <c r="G115" s="28"/>
@@ -9443,20 +9444,20 @@
       <c r="AA115" s="30"/>
       <c r="AB115" s="35"/>
     </row>
-    <row r="116" spans="2:28" s="1" customFormat="1">
+    <row r="116" spans="2:28">
       <c r="B116" s="6"/>
       <c r="C116" s="29"/>
       <c r="D116" s="30"/>
       <c r="E116" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F116" s="65" t="s">
+      <c r="F116" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="G116" s="63"/>
-      <c r="H116" s="64"/>
-      <c r="I116" s="64"/>
-      <c r="J116" s="64"/>
+      <c r="G116" s="57"/>
+      <c r="H116" s="58"/>
+      <c r="I116" s="58"/>
+      <c r="J116" s="58"/>
       <c r="K116" s="30"/>
       <c r="L116" s="30"/>
       <c r="M116" s="30"/>
@@ -9476,14 +9477,14 @@
       <c r="AA116" s="30"/>
       <c r="AB116" s="35"/>
     </row>
-    <row r="117" spans="2:28" s="1" customFormat="1">
+    <row r="117" spans="2:28">
       <c r="B117" s="6"/>
       <c r="C117" s="29"/>
       <c r="D117" s="30"/>
-      <c r="E117" s="59" t="s">
+      <c r="E117" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F117" s="58" t="s">
+      <c r="F117" s="52" t="s">
         <v>51</v>
       </c>
       <c r="G117" s="28"/>
@@ -9509,20 +9510,20 @@
       <c r="AA117" s="30"/>
       <c r="AB117" s="35"/>
     </row>
-    <row r="118" spans="2:28" s="1" customFormat="1">
+    <row r="118" spans="2:28">
       <c r="B118" s="6"/>
       <c r="C118" s="29"/>
       <c r="D118" s="30"/>
       <c r="E118" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F118" s="65" t="s">
+      <c r="F118" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="G118" s="63"/>
-      <c r="H118" s="64"/>
-      <c r="I118" s="64"/>
-      <c r="J118" s="64"/>
+      <c r="G118" s="57"/>
+      <c r="H118" s="58"/>
+      <c r="I118" s="58"/>
+      <c r="J118" s="58"/>
       <c r="K118" s="30"/>
       <c r="L118" s="30"/>
       <c r="M118" s="30"/>
@@ -9542,14 +9543,14 @@
       <c r="AA118" s="30"/>
       <c r="AB118" s="35"/>
     </row>
-    <row r="119" spans="2:28" s="1" customFormat="1">
+    <row r="119" spans="2:28">
       <c r="B119" s="6"/>
       <c r="C119" s="29"/>
       <c r="D119" s="30"/>
-      <c r="E119" s="59" t="s">
+      <c r="E119" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F119" s="58" t="s">
+      <c r="F119" s="52" t="s">
         <v>53</v>
       </c>
       <c r="G119" s="28"/>
@@ -9575,25 +9576,25 @@
       <c r="AA119" s="30"/>
       <c r="AB119" s="35"/>
     </row>
-    <row r="120" spans="2:28" s="1" customFormat="1">
+    <row r="120" spans="2:28">
       <c r="B120" s="6"/>
       <c r="C120" s="29"/>
       <c r="D120" s="30"/>
       <c r="E120" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F120" s="65" t="s">
+      <c r="F120" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="G120" s="63"/>
-      <c r="H120" s="64"/>
-      <c r="I120" s="64"/>
-      <c r="J120" s="64"/>
-      <c r="K120" s="64"/>
-      <c r="L120" s="64"/>
-      <c r="M120" s="64"/>
-      <c r="N120" s="64"/>
-      <c r="O120" s="64"/>
+      <c r="G120" s="57"/>
+      <c r="H120" s="58"/>
+      <c r="I120" s="58"/>
+      <c r="J120" s="58"/>
+      <c r="K120" s="58"/>
+      <c r="L120" s="58"/>
+      <c r="M120" s="58"/>
+      <c r="N120" s="58"/>
+      <c r="O120" s="58"/>
       <c r="P120" s="30"/>
       <c r="Q120" s="30"/>
       <c r="R120" s="30"/>
@@ -9608,7 +9609,7 @@
       <c r="AA120" s="30"/>
       <c r="AB120" s="35"/>
     </row>
-    <row r="121" spans="2:28" s="1" customFormat="1">
+    <row r="121" spans="2:28">
       <c r="B121" s="6"/>
       <c r="C121" s="29"/>
       <c r="D121" s="30"/>
@@ -9637,7 +9638,7 @@
       <c r="AA121" s="30"/>
       <c r="AB121" s="35"/>
     </row>
-    <row r="122" spans="2:28" s="1" customFormat="1">
+    <row r="122" spans="2:28">
       <c r="B122" s="6"/>
       <c r="C122" s="29"/>
       <c r="D122" s="30"/>
@@ -9666,7 +9667,7 @@
       <c r="AA122" s="30"/>
       <c r="AB122" s="35"/>
     </row>
-    <row r="123" spans="2:28" s="1" customFormat="1">
+    <row r="123" spans="2:28">
       <c r="B123" s="6"/>
       <c r="C123" s="29"/>
       <c r="D123" s="30"/>
@@ -9695,7 +9696,7 @@
       <c r="AA123" s="30"/>
       <c r="AB123" s="35"/>
     </row>
-    <row r="124" spans="2:28" s="1" customFormat="1" ht="15.75" thickBot="1">
+    <row r="124" spans="2:28" ht="15.75" thickBot="1">
       <c r="B124" s="38"/>
       <c r="C124" s="39"/>
       <c r="D124" s="40"/>

</xml_diff>